<commit_message>
mau upload and billing report
</commit_message>
<xml_diff>
--- a/billing.xlsx
+++ b/billing.xlsx
@@ -566,7 +566,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,7 +595,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>23 June</t>
+          <t>23 jun 2023</t>
         </is>
       </c>
     </row>
@@ -662,12 +662,12 @@
       <c r="B7" s="10" t="n"/>
       <c r="C7" s="13" t="inlineStr">
         <is>
-          <t>600     Monthly Active Users @601/month</t>
+          <t>600     Monthly Active Users @$601/month</t>
         </is>
       </c>
       <c r="D7" s="13" t="inlineStr">
         <is>
-          <t>23 June</t>
+          <t>23 jun 2023</t>
         </is>
       </c>
       <c r="E7" s="13" t="n">
@@ -682,89 +682,89 @@
       <c r="B8" s="10" t="n"/>
       <c r="C8" s="13" t="inlineStr">
         <is>
-          <t>Additonal Users Outside Tier @$700/per user</t>
+          <t>Platform Support</t>
         </is>
       </c>
       <c r="D8" s="13" t="inlineStr">
         <is>
-          <t>23 June</t>
-        </is>
-      </c>
-      <c r="E8" s="13" t="n">
-        <v>701</v>
-      </c>
+          <t>23 jun 2023</t>
+        </is>
+      </c>
+      <c r="E8" s="13" t="n"/>
       <c r="F8" s="14" t="n">
-        <v>490700</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="n"/>
       <c r="B9" s="10" t="n"/>
-      <c r="C9" s="13" t="inlineStr">
-        <is>
-          <t>800     Agent Seats @801/month</t>
-        </is>
-      </c>
-      <c r="D9" s="13" t="inlineStr">
-        <is>
-          <t>23 June</t>
-        </is>
-      </c>
-      <c r="E9" s="13" t="n">
-        <v>802</v>
-      </c>
-      <c r="F9" s="14" t="n">
-        <v>803</v>
-      </c>
+      <c r="C9" s="9" t="inlineStr">
+        <is>
+          <t>WHATSAPP CONVERSATIONS</t>
+        </is>
+      </c>
+      <c r="D9" s="10" t="n"/>
+      <c r="E9" s="10" t="n"/>
+      <c r="F9" s="10" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="10" t="n"/>
       <c r="B10" s="10" t="n"/>
-      <c r="C10" s="13" t="inlineStr">
-        <is>
-          <t>Platform Support</t>
-        </is>
-      </c>
-      <c r="D10" s="13" t="inlineStr">
-        <is>
-          <t>23 June</t>
-        </is>
-      </c>
-      <c r="E10" s="13" t="n"/>
-      <c r="F10" s="14" t="n">
-        <v>900</v>
+      <c r="C10" s="10" t="inlineStr">
+        <is>
+          <t>Fee Conversation/Month</t>
+        </is>
+      </c>
+      <c r="D10" s="10" t="inlineStr">
+        <is>
+          <t>23 jun 2023</t>
+        </is>
+      </c>
+      <c r="E10" s="15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F10" s="16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="n"/>
       <c r="B11" s="10" t="n"/>
-      <c r="C11" s="9" t="inlineStr">
-        <is>
-          <t>WHATSAPP CONVERSATIONS</t>
-        </is>
-      </c>
-      <c r="D11" s="10" t="n"/>
-      <c r="E11" s="10" t="n"/>
-      <c r="F11" s="10" t="n"/>
+      <c r="C11" s="10" t="inlineStr">
+        <is>
+          <t>Service Conversation</t>
+        </is>
+      </c>
+      <c r="D11" s="10" t="inlineStr">
+        <is>
+          <t>23 jun 2023</t>
+        </is>
+      </c>
+      <c r="E11" s="15" t="n">
+        <v>200</v>
+      </c>
+      <c r="F11" s="16" t="n">
+        <v>201</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="n"/>
       <c r="B12" s="10" t="n"/>
       <c r="C12" s="10" t="inlineStr">
         <is>
-          <t>Fee Conversation/Month</t>
+          <t>Marketing Conversation</t>
         </is>
       </c>
       <c r="D12" s="10" t="inlineStr">
         <is>
-          <t>23 June</t>
+          <t>23 jun 2023</t>
         </is>
       </c>
       <c r="E12" s="15" t="n">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="F12" s="16" t="n">
-        <v>101</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13">
@@ -772,19 +772,19 @@
       <c r="B13" s="10" t="n"/>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>Service Conversation</t>
+          <t>Utility Conversation</t>
         </is>
       </c>
       <c r="D13" s="10" t="inlineStr">
         <is>
-          <t>23 June</t>
+          <t>23 jun 2023</t>
         </is>
       </c>
       <c r="E13" s="15" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F13" s="16" t="n">
-        <v>201</v>
+        <v>401</v>
       </c>
     </row>
     <row r="14">
@@ -792,150 +792,110 @@
       <c r="B14" s="10" t="n"/>
       <c r="C14" s="10" t="inlineStr">
         <is>
-          <t>Marketing Conversation</t>
+          <t>Authentication Conversation</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>23 June</t>
+          <t>23 jun 2023</t>
         </is>
       </c>
       <c r="E14" s="15" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="F14" s="16" t="n">
-        <v>301</v>
+        <v>501</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="10" t="n"/>
-      <c r="B15" s="10" t="n"/>
-      <c r="C15" s="10" t="inlineStr">
-        <is>
-          <t>Utility Conversation</t>
-        </is>
-      </c>
-      <c r="D15" s="10" t="inlineStr">
-        <is>
-          <t>23 June</t>
-        </is>
-      </c>
-      <c r="E15" s="15" t="n">
-        <v>400</v>
-      </c>
-      <c r="F15" s="16" t="n">
-        <v>401</v>
+      <c r="A15" s="17" t="n"/>
+      <c r="B15" s="17" t="n"/>
+      <c r="C15" s="17" t="n"/>
+      <c r="D15" s="17" t="n"/>
+      <c r="E15" s="18" t="inlineStr">
+        <is>
+          <t>Subtotal</t>
+        </is>
+      </c>
+      <c r="F15" s="19" t="n">
+        <v>1703</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="10" t="n"/>
-      <c r="B16" s="10" t="n"/>
-      <c r="C16" s="10" t="inlineStr">
-        <is>
-          <t>Authentication Conversation</t>
-        </is>
-      </c>
-      <c r="D16" s="10" t="inlineStr">
-        <is>
-          <t>23 June</t>
-        </is>
-      </c>
-      <c r="E16" s="15" t="n">
-        <v>500</v>
-      </c>
-      <c r="F16" s="16" t="n">
-        <v>501</v>
+      <c r="A16" s="20" t="inlineStr">
+        <is>
+          <t>ESTIMATED TOTAL</t>
+        </is>
+      </c>
+      <c r="B16" s="21" t="n"/>
+      <c r="C16" s="21" t="n"/>
+      <c r="D16" s="21" t="n"/>
+      <c r="E16" s="21" t="n"/>
+      <c r="F16" s="22" t="n">
+        <v>3.11</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="17" t="n"/>
-      <c r="B17" s="17" t="n"/>
-      <c r="C17" s="17" t="n"/>
-      <c r="D17" s="17" t="n"/>
-      <c r="E17" s="18" t="inlineStr">
-        <is>
-          <t>Subtotal</t>
-        </is>
-      </c>
-      <c r="F17" s="19" t="n">
-        <v>1000</v>
+      <c r="A17" s="20" t="inlineStr">
+        <is>
+          <t>ESTIMATED TOTAL</t>
+        </is>
+      </c>
+      <c r="B17" s="21" t="n"/>
+      <c r="C17" s="21" t="n"/>
+      <c r="D17" s="21" t="n"/>
+      <c r="E17" s="21" t="n"/>
+      <c r="F17" s="23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="20" t="inlineStr">
-        <is>
-          <t>ESTIMATED TOTAL</t>
-        </is>
-      </c>
-      <c r="B18" s="21" t="n"/>
-      <c r="C18" s="21" t="n"/>
-      <c r="D18" s="21" t="n"/>
-      <c r="E18" s="21" t="n"/>
-      <c r="F18" s="22" t="n">
-        <v>3.11</v>
-      </c>
+      <c r="A18" s="24" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="20" t="inlineStr">
-        <is>
-          <t>ESTIMATED TOTAL</t>
-        </is>
-      </c>
-      <c r="B19" s="21" t="n"/>
-      <c r="C19" s="21" t="n"/>
-      <c r="D19" s="21" t="n"/>
-      <c r="E19" s="21" t="n"/>
-      <c r="F19" s="23" t="n">
-        <v>0</v>
+      <c r="A19" s="25" t="inlineStr">
+        <is>
+          <t>Subtotal for clients does not include any line items  billed in PKR. Hence carefully invoice line items in such cases.</t>
+        </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="24" t="n"/>
+      <c r="A20" s="25" t="inlineStr">
+        <is>
+          <t>Estimated totals are provided in USD and PKR seperately where applicable.</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="25" t="inlineStr">
         <is>
-          <t>Subtotal for clients does not include any line items  billed in PKR. Hence carefully invoice line items in such cases.</t>
+          <t>Estimated totals are only provided for billing items chargeable by Eocean hence WhatsApp conversations fee is not included in Estimated totals.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="25" t="inlineStr">
         <is>
-          <t>Estimated totals are provided in USD and PKR seperately where applicable.</t>
+          <t>Verify WhatsApp conversation fee totals from Meta Invoice.</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="25" t="inlineStr">
-        <is>
-          <t>Estimated totals are only provided for billing items chargeable by Eocean hence WhatsApp conversations fee is not included in Estimated totals.</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="25" t="inlineStr">
-        <is>
-          <t>Verify WhatsApp conversation fee totals from Meta Invoice.</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="24" t="n"/>
+      <c r="A23" s="24" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A24:F24"/>
     <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A19:F19"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A19:E19"/>
     <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A18:F18"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A17:E17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>